<commit_message>
add schematron list generator
</commit_message>
<xml_diff>
--- a/docs/extension-complex.xlsx
+++ b/docs/extension-complex.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="89">
   <si>
     <t>Path</t>
   </si>
@@ -281,6 +281,10 @@
   </si>
   <si>
     <t>Extension.extension.valueString</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uri {[]} {[]}
+</t>
   </si>
   <si>
     <t>&lt;valueUri xmlns="http://hl7.org/fhir" value="http://www.fhir.org/guides/test3/StructureDefinition/extension-complex"/&gt;</t>
@@ -1932,7 +1936,7 @@
         <v>37</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="K15" t="s" s="2">
         <v>67</v>
@@ -1949,7 +1953,7 @@
       </c>
       <c r="P15" s="2"/>
       <c r="Q15" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="R15" t="s" s="2">
         <v>37</v>
@@ -2034,7 +2038,7 @@
         <v>37</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K16" t="s" s="2">
         <v>75</v>

</xml_diff>